<commit_message>
Added SMD resistors: 0402 0603 0805 1206 1210 2010 2512
</commit_message>
<xml_diff>
--- a/GOST_Lib/GOST_DbLib.xlsx
+++ b/GOST_Lib/GOST_DbLib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32B86DD-D418-4E92-BCCC-2D73162FC9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17521570-778A-4D37-8BA3-DA12F34A21C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Footprint Path</t>
   </si>
   <si>
-    <t>Resistor</t>
-  </si>
-  <si>
     <t>RES_SMD_0603</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>Library Ref</t>
+  </si>
+  <si>
+    <t>Resistors</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,28 +442,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -474,37 +474,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
       <c r="K2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SMD Ceramic Capasitors: 0402 0603 0805 1206 1210 1812 1825 2220 2225
</commit_message>
<xml_diff>
--- a/GOST_Lib/GOST_DbLib.xlsx
+++ b/GOST_Lib/GOST_DbLib.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17521570-778A-4D37-8BA3-DA12F34A21C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B7B2A-612A-4DC1-9A78-8394515DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6525" yWindow="2250" windowWidth="21600" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors_SMD" sheetId="1" r:id="rId1"/>
+    <sheet name="Capasitors_SMD" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Part Number</t>
   </si>
@@ -42,9 +43,6 @@
     <t>RES_SMD_0603</t>
   </si>
   <si>
-    <t>Resistor.SchLib</t>
-  </si>
-  <si>
     <t>Footprint Ref 2</t>
   </si>
   <si>
@@ -87,7 +85,52 @@
     <t>Library Ref</t>
   </si>
   <si>
-    <t>Resistors</t>
+    <t>Resistors.SchLib</t>
+  </si>
+  <si>
+    <t>Resistor</t>
+  </si>
+  <si>
+    <t>CAP_SMD_0402</t>
+  </si>
+  <si>
+    <t>CAP_SMD_0603</t>
+  </si>
+  <si>
+    <t>CAP_SMD_0805</t>
+  </si>
+  <si>
+    <t>CAP_SMD_1206</t>
+  </si>
+  <si>
+    <t>CAP_SMD_1210</t>
+  </si>
+  <si>
+    <t>CAP_SMD_1812</t>
+  </si>
+  <si>
+    <t>Footprint Ref 8</t>
+  </si>
+  <si>
+    <t>Footprint Ref 9</t>
+  </si>
+  <si>
+    <t>CAP_SMD_1825</t>
+  </si>
+  <si>
+    <t>CAP_SMD_2220</t>
+  </si>
+  <si>
+    <t>CAP_SMD_2225</t>
+  </si>
+  <si>
+    <t>Capacitors.SchLib</t>
+  </si>
+  <si>
+    <t>CAP_SMD.PcbLib</t>
+  </si>
+  <si>
+    <t>Capacitor</t>
   </si>
 </sst>
 </file>
@@ -420,9 +463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,28 +485,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>2</v>
@@ -480,31 +523,138 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
         <v>14</v>
       </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4164A9E-FF46-467E-B380-FA61312CCDD8}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Tantalum SMD Capacitors sizes: A B C D E V
</commit_message>
<xml_diff>
--- a/GOST_Lib/GOST_DbLib.xlsx
+++ b/GOST_Lib/GOST_DbLib.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E63B7B2A-612A-4DC1-9A78-8394515DD0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D3299F-4365-41A1-B32E-068E9CF524C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="2250" windowWidth="21600" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6525" yWindow="2250" windowWidth="21600" windowHeight="11475" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors_SMD" sheetId="1" r:id="rId1"/>
-    <sheet name="Capasitors_SMD" sheetId="2" r:id="rId2"/>
+    <sheet name="Capacitors_SMD" sheetId="2" r:id="rId2"/>
+    <sheet name="Tantalum_Capacitors_SMD" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Part Number</t>
   </si>
@@ -131,6 +132,33 @@
   </si>
   <si>
     <t>Capacitor</t>
+  </si>
+  <si>
+    <t>Tantalum Capacitor</t>
+  </si>
+  <si>
+    <t>Polarized Capacitor</t>
+  </si>
+  <si>
+    <t>CAP_SMD_TANTALUM.PcbLib</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_A</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_B</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_C</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_D</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_E</t>
+  </si>
+  <si>
+    <t>TANT_CAP_SMD_V</t>
   </si>
 </sst>
 </file>
@@ -475,7 +503,7 @@
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -560,9 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4164A9E-FF46-467E-B380-FA61312CCDD8}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,4 +689,94 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1AF6E3-E00B-4FA8-802B-A00B294F4270}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>